<commit_message>
DUMMY PORFTOKOLIO PL FILES ADDED
</commit_message>
<xml_diff>
--- a/LOT_MGMT/Equity_Transaction_Summary_1jan2025to13may2025.xlsx
+++ b/LOT_MGMT/Equity_Transaction_Summary_1jan2025to13may2025.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions Summary" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7566" uniqueCount="1540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7629" uniqueCount="1540">
   <si>
     <t xml:space="preserve">Stock Name</t>
   </si>
@@ -5263,8 +5264,8 @@
   </sheetPr>
   <dimension ref="A1:S1192"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A171" activeCellId="0" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -58118,4 +58119,455 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="16" t="n">
+        <v>81.54</v>
+      </c>
+      <c r="H2" s="16" t="n">
+        <v>407.7</v>
+      </c>
+      <c r="I2" s="16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="16" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K2" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="16" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="M2" s="16" t="n">
+        <v>358</v>
+      </c>
+      <c r="N2" s="17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="16" t="n">
+        <v>761</v>
+      </c>
+      <c r="G3" s="16" t="n">
+        <v>81.56</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="16" t="n">
+        <v>15.22</v>
+      </c>
+      <c r="J3" s="16" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="K3" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16" t="n">
+        <v>9.39</v>
+      </c>
+      <c r="M3" s="16" t="n">
+        <v>358</v>
+      </c>
+      <c r="N3" s="17" t="n">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="16" t="n">
+        <v>234</v>
+      </c>
+      <c r="G4" s="16" t="n">
+        <v>81.57</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I4" s="16" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="J4" s="16" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="K4" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="M4" s="16" t="n">
+        <v>358</v>
+      </c>
+      <c r="N4" s="17" t="n">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5" s="0" t="n">
+        <f aca="false">I2+I3+I4</f>
+        <v>20</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">J2+J3+J4</f>
+        <v>3.6</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">K2+K3+K4</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">L2+L3+L4</f>
+        <v>12.33</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>500</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>79.19</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="M6" s="11" t="n">
+        <v>363</v>
+      </c>
+      <c r="N6" s="12" t="n">
+        <v>500</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="G7" s="16" t="n">
+        <v>81.44</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="I7" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J7" s="16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M7" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" s="16" t="n">
+        <v>82.56</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" s="16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K8" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="M8" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="16" t="n">
+        <v>50</v>
+      </c>
+      <c r="G10" s="16" t="n">
+        <v>302.84</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J10" s="16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K10" s="16" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="L10" s="16" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="M10" s="16" t="n">
+        <v>357</v>
+      </c>
+      <c r="N10" s="17" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>261</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="16" t="n">
+        <v>100</v>
+      </c>
+      <c r="G11" s="16" t="n">
+        <v>154.49</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="I11" s="16" t="n">
+        <v>20</v>
+      </c>
+      <c r="J11" s="16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="K11" s="16" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="L11" s="16" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>